<commit_message>
Referencias para trabajar INEE
</commit_message>
<xml_diff>
--- a/Finanzas/2_Mayo-Ago_2018.xlsx
+++ b/Finanzas/2_Mayo-Ago_2018.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prestamo\Desktop\Adrifelcha_Lab25\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="180">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -487,11 +487,89 @@
   <si>
     <t>Capuchino</t>
   </si>
+  <si>
+    <t>PRIMER DIA INEE</t>
+  </si>
+  <si>
+    <t>Papeles INEE</t>
+  </si>
+  <si>
+    <t>Ultima clase Emiliano</t>
+  </si>
+  <si>
+    <t>Emiliano</t>
+  </si>
+  <si>
+    <t>Cumple Jaime!</t>
+  </si>
+  <si>
+    <t>Wingstop</t>
+  </si>
+  <si>
+    <t>Hooters</t>
+  </si>
+  <si>
+    <t>Cita Nariz</t>
+  </si>
+  <si>
+    <t>Kari Feliciano proyecto</t>
+  </si>
+  <si>
+    <t>Sushi</t>
+  </si>
+  <si>
+    <t>Fridays</t>
+  </si>
+  <si>
+    <t>Frapuchino</t>
+  </si>
+  <si>
+    <t>Carnitas</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>Tarjeta Jaime; Cervezas</t>
+  </si>
+  <si>
+    <t>Compras</t>
+  </si>
+  <si>
+    <t>Microporo y Toallas</t>
+  </si>
+  <si>
+    <t>Jaime Justice League final</t>
+  </si>
+  <si>
+    <t>casa</t>
+  </si>
+  <si>
+    <t>Entrevista INEE</t>
+  </si>
+  <si>
+    <t>Clase Emiliano</t>
+  </si>
+  <si>
+    <t>Deposito Ale; Fotos infantiles; Taxis; Taxi a casa de Mariana</t>
+  </si>
+  <si>
+    <t>JL invito</t>
+  </si>
+  <si>
+    <t>Deadpool 2</t>
+  </si>
+  <si>
+    <t>Ale Deposito Trabajo</t>
+  </si>
+  <si>
+    <t>Boletos de Cine</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1351,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,7 +1507,7 @@
       <c r="E2" s="56"/>
       <c r="F2" s="112">
         <f>N3-D2</f>
-        <v>-5060</v>
+        <v>-7310</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>2</v>
@@ -1556,7 +1634,7 @@
       </c>
       <c r="N3" s="25">
         <f>(SUM(D2,(K11:K499)))-(SUM((J11:J499),(I11:I499)))</f>
-        <v>2703</v>
+        <v>453</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
@@ -1639,7 +1717,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>38137</v>
+        <v>35875</v>
       </c>
       <c r="Z4" s="47">
         <v>43222</v>
@@ -1707,7 +1785,7 @@
       </c>
       <c r="BG4" s="57">
         <f>(SUM((AV3:AV519)))-(SUM((AZ3:AZ519)))</f>
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="BH4" s="57"/>
     </row>
@@ -1809,7 +1887,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I499)))-(SUM((X11:X499)))</f>
-        <v>1614</v>
+        <v>1602</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -1893,7 +1971,7 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>1614</v>
+        <v>1602</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
@@ -2200,18 +2278,27 @@
       <c r="AA10" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="AB10" s="49"/>
+      <c r="AB10" s="49" t="s">
+        <v>174</v>
+      </c>
       <c r="AC10" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD10" s="50"/>
+        <v>10</v>
+      </c>
+      <c r="AD10" s="50">
+        <v>80</v>
+      </c>
       <c r="AE10" s="50"/>
       <c r="AG10" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI10" s="98"/>
+        <v>70</v>
+      </c>
+      <c r="AH10">
+        <v>70</v>
+      </c>
+      <c r="AI10" s="98" t="s">
+        <v>115</v>
+      </c>
       <c r="AJ10" s="56"/>
       <c r="AK10" s="56"/>
       <c r="AL10" s="56"/>
@@ -2303,20 +2390,33 @@
       <c r="AA11" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="AB11" s="49"/>
+      <c r="AB11" s="49" t="s">
+        <v>158</v>
+      </c>
       <c r="AC11" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD11" s="50"/>
+        <v>-720</v>
+      </c>
+      <c r="AD11" s="50">
+        <v>80</v>
+      </c>
       <c r="AE11" s="50"/>
       <c r="AG11" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI11" s="98"/>
-      <c r="AJ11" s="56"/>
-      <c r="AK11" s="56"/>
+        <v>800</v>
+      </c>
+      <c r="AH11">
+        <v>400</v>
+      </c>
+      <c r="AI11" s="98" t="s">
+        <v>159</v>
+      </c>
+      <c r="AJ11" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="AK11" s="56">
+        <v>400</v>
+      </c>
       <c r="AL11" s="56"/>
       <c r="AM11" s="56"/>
       <c r="AN11" s="56"/>
@@ -2410,20 +2510,33 @@
       <c r="AA12" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="AB12" s="49"/>
+      <c r="AB12" s="49" t="s">
+        <v>161</v>
+      </c>
       <c r="AC12" s="41">
         <f>(SUM(AD12,AE12))-AG12</f>
-        <v>0</v>
-      </c>
-      <c r="AD12" s="50"/>
+        <v>-70</v>
+      </c>
+      <c r="AD12" s="50">
+        <v>70</v>
+      </c>
       <c r="AE12" s="110"/>
       <c r="AG12" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI12" s="98"/>
-      <c r="AJ12" s="56"/>
-      <c r="AK12" s="56"/>
+        <v>140</v>
+      </c>
+      <c r="AH12">
+        <v>70</v>
+      </c>
+      <c r="AI12" s="98" t="s">
+        <v>165</v>
+      </c>
+      <c r="AJ12" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK12" s="56">
+        <v>40</v>
+      </c>
       <c r="AL12" s="56"/>
       <c r="AM12" s="56"/>
       <c r="AN12" s="56"/>
@@ -2435,15 +2548,21 @@
       <c r="AT12" s="56"/>
       <c r="AU12">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AV12" s="56"/>
-      <c r="AW12" s="56"/>
+        <v>30</v>
+      </c>
+      <c r="AV12" s="56">
+        <v>30</v>
+      </c>
+      <c r="AW12" s="56">
+        <v>1</v>
+      </c>
       <c r="AX12" s="56"/>
-      <c r="AY12" s="56"/>
+      <c r="AY12" s="56">
+        <v>2</v>
+      </c>
       <c r="AZ12" s="56">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="BA12" s="56"/>
       <c r="BB12">
@@ -2516,18 +2635,27 @@
       <c r="AA13" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="AB13" s="49"/>
+      <c r="AB13" s="49" t="s">
+        <v>162</v>
+      </c>
       <c r="AC13" s="41">
         <f>(SUM(AD13,AE13))-AG13</f>
-        <v>0</v>
-      </c>
-      <c r="AD13" s="50"/>
+        <v>-70</v>
+      </c>
+      <c r="AD13" s="50">
+        <v>80</v>
+      </c>
       <c r="AE13" s="50"/>
       <c r="AG13" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI13" s="98"/>
+        <v>150</v>
+      </c>
+      <c r="AH13">
+        <v>150</v>
+      </c>
+      <c r="AI13" s="98" t="s">
+        <v>164</v>
+      </c>
       <c r="AJ13" s="56"/>
       <c r="AK13" s="123"/>
       <c r="AL13" s="56"/>
@@ -2597,10 +2725,16 @@
         <f t="shared" si="6"/>
         <v>600</v>
       </c>
-      <c r="T14" s="36"/>
-      <c r="U14" s="57"/>
+      <c r="T14" s="36">
+        <v>43228</v>
+      </c>
+      <c r="U14" s="57" t="s">
+        <v>157</v>
+      </c>
       <c r="V14" s="35"/>
-      <c r="W14" s="37"/>
+      <c r="W14" s="37">
+        <v>100</v>
+      </c>
       <c r="X14" s="37"/>
       <c r="Z14" s="47">
         <v>43232</v>
@@ -2608,20 +2742,33 @@
       <c r="AA14" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="AB14" s="49"/>
+      <c r="AB14" s="49" t="s">
+        <v>171</v>
+      </c>
       <c r="AC14" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD14" s="50"/>
+        <v>50</v>
+      </c>
+      <c r="AD14" s="50">
+        <v>200</v>
+      </c>
       <c r="AE14" s="50"/>
       <c r="AG14" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI14" s="98"/>
-      <c r="AJ14" s="56"/>
-      <c r="AK14" s="56"/>
+        <v>150</v>
+      </c>
+      <c r="AH14">
+        <v>100</v>
+      </c>
+      <c r="AI14" s="98" t="s">
+        <v>167</v>
+      </c>
+      <c r="AJ14" s="56" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK14" s="56">
+        <v>50</v>
+      </c>
       <c r="AL14" s="56"/>
       <c r="AM14" s="56"/>
       <c r="AN14" s="56"/>
@@ -2663,9 +2810,15 @@
         <f t="shared" si="5"/>
         <v>1300</v>
       </c>
-      <c r="G15" s="97"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
+      <c r="G15" s="97">
+        <v>43236</v>
+      </c>
+      <c r="H15" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="I15" s="56">
+        <v>2100</v>
+      </c>
       <c r="J15" s="56"/>
       <c r="K15" s="56"/>
       <c r="M15" s="18"/>
@@ -2683,10 +2836,16 @@
         <f>P15-Q15</f>
         <v>1000</v>
       </c>
-      <c r="T15" s="36"/>
-      <c r="U15" s="35"/>
+      <c r="T15" s="36">
+        <v>43234</v>
+      </c>
+      <c r="U15" s="35" t="s">
+        <v>157</v>
+      </c>
       <c r="V15" s="35"/>
-      <c r="W15" s="37"/>
+      <c r="W15" s="37">
+        <v>200</v>
+      </c>
       <c r="X15" s="37"/>
       <c r="Z15" s="47">
         <v>43233</v>
@@ -2694,15 +2853,22 @@
       <c r="AA15" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="AB15" s="72"/>
+      <c r="AB15" s="72" t="s">
+        <v>172</v>
+      </c>
       <c r="AC15" s="41">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AD15" s="50"/>
+      <c r="AD15" s="50">
+        <v>0</v>
+      </c>
       <c r="AE15" s="50"/>
       <c r="AG15" s="51">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH15">
         <v>0</v>
       </c>
       <c r="AI15" s="56"/>
@@ -2740,10 +2906,16 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G16" s="97"/>
-      <c r="H16" s="56"/>
+      <c r="G16" s="97">
+        <v>43237</v>
+      </c>
+      <c r="H16" s="56" t="s">
+        <v>179</v>
+      </c>
       <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
+      <c r="J16" s="56">
+        <v>150</v>
+      </c>
       <c r="K16" s="56"/>
       <c r="M16" s="18"/>
       <c r="N16" s="18" t="s">
@@ -2760,10 +2932,16 @@
         <f t="shared" si="6"/>
         <v>120</v>
       </c>
-      <c r="T16" s="36"/>
-      <c r="U16" s="35"/>
+      <c r="T16" s="36">
+        <v>43236</v>
+      </c>
+      <c r="U16" s="35" t="s">
+        <v>127</v>
+      </c>
       <c r="V16" s="35"/>
-      <c r="W16" s="37"/>
+      <c r="W16" s="37">
+        <v>500</v>
+      </c>
       <c r="X16" s="37"/>
       <c r="Z16" s="47">
         <v>43234</v>
@@ -2771,21 +2949,41 @@
       <c r="AA16" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="AB16" s="49"/>
+      <c r="AB16" s="49" t="s">
+        <v>156</v>
+      </c>
       <c r="AC16" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD16" s="50"/>
-      <c r="AE16" s="50"/>
+        <v>38</v>
+      </c>
+      <c r="AD16" s="50">
+        <v>120</v>
+      </c>
+      <c r="AE16" s="50">
+        <v>200</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>169</v>
+      </c>
       <c r="AG16" s="68">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI16" s="56"/>
-      <c r="AJ16" s="56"/>
-      <c r="AK16" s="56"/>
-      <c r="AL16" s="56"/>
+        <v>282</v>
+      </c>
+      <c r="AH16">
+        <v>50</v>
+      </c>
+      <c r="AI16" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="AJ16" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AK16" s="56">
+        <v>80</v>
+      </c>
+      <c r="AL16" s="56">
+        <v>130</v>
+      </c>
       <c r="AM16" s="56"/>
       <c r="AN16" s="56"/>
       <c r="AO16" s="56"/>
@@ -2796,15 +2994,21 @@
       <c r="AT16" s="56"/>
       <c r="AU16">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AV16" s="56"/>
-      <c r="AW16" s="56"/>
+        <v>22</v>
+      </c>
+      <c r="AV16" s="56">
+        <v>22</v>
+      </c>
+      <c r="AW16" s="56">
+        <v>2</v>
+      </c>
       <c r="AX16" s="56"/>
-      <c r="AY16" s="56"/>
+      <c r="AY16" s="56">
+        <v>2</v>
+      </c>
       <c r="AZ16" s="56">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="BA16" s="56"/>
       <c r="BB16">
@@ -2848,18 +3052,27 @@
       <c r="AA17" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="AB17" s="49"/>
+      <c r="AB17" s="49" t="s">
+        <v>173</v>
+      </c>
       <c r="AC17" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD17" s="50"/>
+        <v>-85</v>
+      </c>
+      <c r="AD17" s="50">
+        <v>80</v>
+      </c>
       <c r="AE17" s="67"/>
       <c r="AG17" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI17" s="56"/>
+        <v>165</v>
+      </c>
+      <c r="AH17">
+        <v>150</v>
+      </c>
+      <c r="AI17" s="56" t="s">
+        <v>163</v>
+      </c>
       <c r="AJ17" s="98"/>
       <c r="AK17" s="56"/>
       <c r="AL17" s="56"/>
@@ -2873,7 +3086,7 @@
       <c r="AT17" s="56"/>
       <c r="AU17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AV17" s="56"/>
       <c r="AW17" s="56"/>
@@ -2883,10 +3096,12 @@
         <f>(AW17*8)+(AY17*5)</f>
         <v>0</v>
       </c>
-      <c r="BA17" s="56"/>
+      <c r="BA17" s="56">
+        <v>3</v>
+      </c>
       <c r="BB17">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:60" x14ac:dyDescent="0.25">
@@ -2925,23 +3140,42 @@
       <c r="AA18" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="AB18" s="72"/>
+      <c r="AB18" s="72" t="s">
+        <v>155</v>
+      </c>
       <c r="AC18" s="69">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD18" s="50"/>
+        <v>-2265</v>
+      </c>
+      <c r="AD18" s="50">
+        <v>80</v>
+      </c>
       <c r="AE18" s="50"/>
       <c r="AG18" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI18" s="56"/>
-      <c r="AJ18" s="98"/>
-      <c r="AK18" s="56"/>
-      <c r="AL18" s="56"/>
-      <c r="AM18" s="56"/>
-      <c r="AN18" s="56"/>
+        <v>2345</v>
+      </c>
+      <c r="AH18">
+        <v>85</v>
+      </c>
+      <c r="AI18" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ18" s="98" t="s">
+        <v>175</v>
+      </c>
+      <c r="AK18" s="100">
+        <v>2100</v>
+      </c>
+      <c r="AL18" s="56">
+        <v>50</v>
+      </c>
+      <c r="AM18" s="56">
+        <v>50</v>
+      </c>
+      <c r="AN18" s="56">
+        <v>50</v>
+      </c>
       <c r="AO18" s="56"/>
       <c r="AP18" s="56"/>
       <c r="AQ18" s="56"/>
@@ -2950,7 +3184,7 @@
       <c r="AT18" s="56"/>
       <c r="AU18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AV18" s="56"/>
       <c r="AW18" s="56"/>
@@ -2960,10 +3194,12 @@
         <f>(AW18*8)+(AY18*5)</f>
         <v>0</v>
       </c>
-      <c r="BA18" s="56"/>
+      <c r="BA18" s="56">
+        <v>2</v>
+      </c>
       <c r="BB18">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:60" x14ac:dyDescent="0.25">
@@ -3002,19 +3238,28 @@
       <c r="AA19" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="AB19" s="49"/>
+      <c r="AB19" s="49" t="s">
+        <v>154</v>
+      </c>
       <c r="AC19" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD19" s="50"/>
+        <v>140</v>
+      </c>
+      <c r="AD19" s="50">
+        <v>150</v>
+      </c>
       <c r="AE19" s="50"/>
       <c r="AG19" s="51">
         <f>SUM(AH19,AJ19,AK19,AL19,AM19,AN19,AP19,AQ19,AR19,AS19,AT19,AU19)</f>
-        <v>0</v>
-      </c>
-      <c r="AI19" s="56"/>
-      <c r="AJ19" s="56"/>
+        <v>10</v>
+      </c>
+      <c r="AH19">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="AJ19" s="98"/>
       <c r="AK19" s="56"/>
       <c r="AL19" s="56"/>
       <c r="AM19" s="56"/>
@@ -3027,7 +3272,7 @@
       <c r="AT19" s="56"/>
       <c r="AU19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AV19" s="107"/>
       <c r="AW19" s="56"/>
@@ -3037,10 +3282,12 @@
         <f>(AW19*8)+(AY19*5)</f>
         <v>0</v>
       </c>
-      <c r="BA19" s="56"/>
+      <c r="BA19" s="56">
+        <v>2</v>
+      </c>
       <c r="BB19">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BH19" s="38"/>
     </row>
@@ -3080,20 +3327,28 @@
       <c r="AA20" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="AB20" s="49"/>
+      <c r="AB20" s="49" t="s">
+        <v>177</v>
+      </c>
       <c r="AC20" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD20" s="50"/>
+        <v>60</v>
+      </c>
+      <c r="AD20" s="50">
+        <v>100</v>
+      </c>
       <c r="AE20" s="50"/>
       <c r="AG20" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AI20" s="56"/>
-      <c r="AJ20" s="98"/>
-      <c r="AK20" s="56"/>
+      <c r="AJ20" s="98" t="s">
+        <v>153</v>
+      </c>
+      <c r="AK20" s="56">
+        <v>30</v>
+      </c>
       <c r="AL20" s="56"/>
       <c r="AM20" s="56"/>
       <c r="AN20" s="56"/>
@@ -3105,7 +3360,7 @@
       <c r="AT20" s="56"/>
       <c r="AU20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AV20" s="56"/>
       <c r="AW20" s="56"/>
@@ -3115,10 +3370,12 @@
         <f>(AW20*6)+(AX20*8)+(AY20*5)</f>
         <v>0</v>
       </c>
-      <c r="BA20" s="56"/>
+      <c r="BA20" s="56">
+        <v>2</v>
+      </c>
       <c r="BB20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finanzas y capitulo Michael Lee
</commit_message>
<xml_diff>
--- a/Finanzas/2_Mayo-Ago_2018.xlsx
+++ b/Finanzas/2_Mayo-Ago_2018.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="188">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -564,6 +564,30 @@
   </si>
   <si>
     <t>Boletos de Cine</t>
+  </si>
+  <si>
+    <t>Deposito Amigo</t>
+  </si>
+  <si>
+    <t>Kura con papás</t>
+  </si>
+  <si>
+    <t>Vallet Parking</t>
+  </si>
+  <si>
+    <t>Primera semana</t>
+  </si>
+  <si>
+    <t>Compra sacos y pantalones</t>
+  </si>
+  <si>
+    <t>Taco Beef con Jaime</t>
+  </si>
+  <si>
+    <t>Udon</t>
+  </si>
+  <si>
+    <t>Capuchino y Americano</t>
   </si>
 </sst>
 </file>
@@ -1207,7 +1231,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1242,7 +1266,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1429,8 +1453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="X15" workbookViewId="0">
+      <selection activeCell="AJ24" sqref="AJ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,7 +1741,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>35875</v>
+        <v>37175</v>
       </c>
       <c r="Z4" s="47">
         <v>43222</v>
@@ -1887,7 +1911,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I499)))-(SUM((X11:X499)))</f>
-        <v>1602</v>
+        <v>802</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -1971,7 +1995,7 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>1602</v>
+        <v>802</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
@@ -2133,7 +2157,7 @@
       </c>
       <c r="R9" s="15">
         <f>SUM(R11:R481)</f>
-        <v>33820</v>
+        <v>35920</v>
       </c>
       <c r="T9" s="32" t="s">
         <v>40</v>
@@ -3332,7 +3356,7 @@
       </c>
       <c r="AC20" s="41">
         <f t="shared" si="3"/>
-        <v>60</v>
+        <v>-90</v>
       </c>
       <c r="AD20" s="50">
         <v>100</v>
@@ -3340,9 +3364,14 @@
       <c r="AE20" s="50"/>
       <c r="AG20" s="51">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="AI20" s="56"/>
+        <v>190</v>
+      </c>
+      <c r="AH20">
+        <v>150</v>
+      </c>
+      <c r="AI20" s="56" t="s">
+        <v>185</v>
+      </c>
       <c r="AJ20" s="98" t="s">
         <v>153</v>
       </c>
@@ -3414,20 +3443,31 @@
       <c r="AA21" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="AB21" s="49"/>
+      <c r="AB21" s="49" t="s">
+        <v>181</v>
+      </c>
       <c r="AC21" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-550</v>
       </c>
       <c r="AD21" s="50"/>
       <c r="AE21" s="70"/>
       <c r="AG21" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI21" s="98"/>
-      <c r="AJ21" s="98"/>
-      <c r="AK21" s="98"/>
+        <v>550</v>
+      </c>
+      <c r="AH21">
+        <v>500</v>
+      </c>
+      <c r="AI21" s="98" t="s">
+        <v>181</v>
+      </c>
+      <c r="AJ21" s="98" t="s">
+        <v>182</v>
+      </c>
+      <c r="AK21" s="98">
+        <v>50</v>
+      </c>
       <c r="AL21" s="56"/>
       <c r="AM21" s="56"/>
       <c r="AN21" s="56"/>
@@ -3491,20 +3531,29 @@
       <c r="AA22" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="AB22" s="49"/>
+      <c r="AB22" s="49" t="s">
+        <v>184</v>
+      </c>
       <c r="AC22" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-50</v>
       </c>
       <c r="AD22" s="67"/>
       <c r="AE22" s="67"/>
       <c r="AG22" s="51">
         <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="AH22">
         <v>0</v>
       </c>
       <c r="AI22" s="56"/>
-      <c r="AJ22" s="56"/>
-      <c r="AK22" s="56"/>
+      <c r="AJ22" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK22" s="56">
+        <v>50</v>
+      </c>
       <c r="AL22" s="56"/>
       <c r="AM22" s="56"/>
       <c r="AN22" s="56"/>
@@ -3569,21 +3618,36 @@
       <c r="AA23" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="AB23" s="49"/>
+      <c r="AB23" s="49" t="s">
+        <v>183</v>
+      </c>
       <c r="AC23" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD23" s="50"/>
+        <v>-50</v>
+      </c>
+      <c r="AD23" s="50">
+        <v>170</v>
+      </c>
       <c r="AE23" s="50"/>
       <c r="AG23" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI23" s="56"/>
-      <c r="AJ23" s="56"/>
-      <c r="AK23" s="56"/>
-      <c r="AL23" s="107"/>
+        <v>220</v>
+      </c>
+      <c r="AH23">
+        <v>160</v>
+      </c>
+      <c r="AI23" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="AJ23" s="56" t="s">
+        <v>187</v>
+      </c>
+      <c r="AK23" s="56">
+        <v>30</v>
+      </c>
+      <c r="AL23" s="107">
+        <v>20</v>
+      </c>
       <c r="AM23" s="56"/>
       <c r="AN23" s="56"/>
       <c r="AO23" s="56"/>
@@ -3594,7 +3658,7 @@
       <c r="AT23" s="56"/>
       <c r="AU23" s="38">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AV23" s="56"/>
       <c r="AW23" s="56"/>
@@ -3604,10 +3668,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BA23" s="56"/>
+      <c r="BA23" s="56">
+        <v>2</v>
+      </c>
       <c r="BB23">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:60" x14ac:dyDescent="0.25">
@@ -4643,14 +4709,22 @@
       <c r="I37" s="99"/>
       <c r="J37" s="100"/>
       <c r="K37" s="101"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="23"/>
+      <c r="M37" s="59">
+        <v>43236</v>
+      </c>
+      <c r="N37" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="O37" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="P37" s="23">
+        <v>2100</v>
+      </c>
       <c r="Q37" s="22"/>
       <c r="R37" s="20">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2100</v>
       </c>
       <c r="T37" s="36"/>
       <c r="U37" s="35"/>

</xml_diff>

<commit_message>
Martes 22 de mayo
</commit_message>
<xml_diff>
--- a/Finanzas/2_Mayo-Ago_2018.xlsx
+++ b/Finanzas/2_Mayo-Ago_2018.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="190">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -587,7 +587,13 @@
     <t>Udon</t>
   </si>
   <si>
-    <t>Capuchino y Americano</t>
+    <t>Comida Corrida</t>
+  </si>
+  <si>
+    <t>Comida Corrida JL</t>
+  </si>
+  <si>
+    <t>Capuchino, Americano, Metrobus JL y Tarjeta Metro</t>
   </si>
 </sst>
 </file>
@@ -1453,8 +1459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X15" workbookViewId="0">
-      <selection activeCell="AJ24" sqref="AJ24"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,7 +1747,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>37175</v>
+        <v>37552</v>
       </c>
       <c r="Z4" s="47">
         <v>43222</v>
@@ -1809,7 +1815,7 @@
       </c>
       <c r="BG4" s="57">
         <f>(SUM((AV3:AV519)))-(SUM((AZ3:AZ519)))</f>
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="BH4" s="57"/>
     </row>
@@ -1911,7 +1917,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I499)))-(SUM((X11:X499)))</f>
-        <v>802</v>
+        <v>1179</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -1995,7 +2001,7 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>802</v>
+        <v>1179</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
@@ -3623,7 +3629,7 @@
       </c>
       <c r="AC23" s="41">
         <f t="shared" si="3"/>
-        <v>-50</v>
+        <v>-115</v>
       </c>
       <c r="AD23" s="50">
         <v>170</v>
@@ -3631,7 +3637,7 @@
       <c r="AE23" s="50"/>
       <c r="AG23" s="51">
         <f t="shared" si="0"/>
-        <v>220</v>
+        <v>285</v>
       </c>
       <c r="AH23">
         <v>160</v>
@@ -3640,7 +3646,7 @@
         <v>186</v>
       </c>
       <c r="AJ23" s="56" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AK23" s="56">
         <v>30</v>
@@ -3648,7 +3654,9 @@
       <c r="AL23" s="107">
         <v>20</v>
       </c>
-      <c r="AM23" s="56"/>
+      <c r="AM23" s="56">
+        <v>15</v>
+      </c>
       <c r="AN23" s="56"/>
       <c r="AO23" s="56"/>
       <c r="AP23" s="56"/>
@@ -3658,15 +3666,19 @@
       <c r="AT23" s="56"/>
       <c r="AU23" s="38">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="AV23" s="56"/>
+        <v>60</v>
+      </c>
+      <c r="AV23" s="56">
+        <v>50</v>
+      </c>
       <c r="AW23" s="56"/>
       <c r="AX23" s="56"/>
-      <c r="AY23" s="56"/>
+      <c r="AY23" s="56">
+        <v>1</v>
+      </c>
       <c r="AZ23" s="56">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BA23" s="56">
         <v>2</v>
@@ -3714,20 +3726,33 @@
       <c r="AA24" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="AB24" s="119"/>
+      <c r="AB24" s="119" t="s">
+        <v>188</v>
+      </c>
       <c r="AC24" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD24" s="50"/>
+        <v>442</v>
+      </c>
+      <c r="AD24" s="50">
+        <v>600</v>
+      </c>
       <c r="AE24" s="50"/>
       <c r="AG24" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI24" s="56"/>
-      <c r="AJ24" s="56"/>
-      <c r="AK24" s="56"/>
+        <v>158</v>
+      </c>
+      <c r="AH24">
+        <v>128</v>
+      </c>
+      <c r="AI24" s="56" t="s">
+        <v>187</v>
+      </c>
+      <c r="AJ24" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="AK24" s="56">
+        <v>30</v>
+      </c>
       <c r="AL24" s="93"/>
       <c r="AM24" s="56"/>
       <c r="AN24" s="56"/>
@@ -3744,10 +3769,12 @@
       <c r="AV24" s="56"/>
       <c r="AW24" s="107"/>
       <c r="AX24" s="56"/>
-      <c r="AY24" s="56"/>
+      <c r="AY24" s="56">
+        <v>2</v>
+      </c>
       <c r="AZ24" s="56">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BA24" s="56"/>
       <c r="BB24">

</xml_diff>

<commit_message>
Gastos cena con Jaime
</commit_message>
<xml_diff>
--- a/Finanzas/2_Mayo-Ago_2018.xlsx
+++ b/Finanzas/2_Mayo-Ago_2018.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="191">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -595,6 +595,9 @@
   <si>
     <t>Capuchino, Americano, Metrobus JL y Tarjeta Metro</t>
   </si>
+  <si>
+    <t>Capuchino y Chillis con Jaime</t>
+  </si>
 </sst>
 </file>
 
@@ -754,7 +757,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="32">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -941,6 +944,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -954,7 +963,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1163,6 +1172,7 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1171,8 +1181,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD52F8E"/>
       <color rgb="FF33CC33"/>
-      <color rgb="FFD52F8E"/>
       <color rgb="FFFF9797"/>
       <color rgb="FFFF00FF"/>
       <color rgb="FF99FF99"/>
@@ -1460,7 +1470,7 @@
   <dimension ref="A1:BH963"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1709,12 +1719,16 @@
         <v>6</v>
       </c>
       <c r="AV3" s="56"/>
-      <c r="AW3" s="56"/>
-      <c r="AX3" s="56"/>
-      <c r="AY3" s="56"/>
+      <c r="AW3" s="124">
+        <v>4</v>
+      </c>
+      <c r="AX3" s="124"/>
+      <c r="AY3" s="124">
+        <v>5</v>
+      </c>
       <c r="AZ3" s="56">
         <f t="shared" ref="AZ3:AZ16" si="2">(AW3*6)+(AY3*5)</f>
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="BA3" s="56"/>
       <c r="BB3">
@@ -1747,7 +1761,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>37552</v>
+        <v>37332</v>
       </c>
       <c r="Z4" s="47">
         <v>43222</v>
@@ -1815,7 +1829,7 @@
       </c>
       <c r="BG4" s="57">
         <f>(SUM((AV3:AV519)))-(SUM((AZ3:AZ519)))</f>
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="BH4" s="57"/>
     </row>
@@ -1917,7 +1931,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I499)))-(SUM((X11:X499)))</f>
-        <v>1179</v>
+        <v>959</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -2001,7 +2015,7 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>1179</v>
+        <v>959</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
@@ -3731,7 +3745,7 @@
       </c>
       <c r="AC24" s="41">
         <f t="shared" si="3"/>
-        <v>442</v>
+        <v>222</v>
       </c>
       <c r="AD24" s="50">
         <v>600</v>
@@ -3739,7 +3753,7 @@
       <c r="AE24" s="50"/>
       <c r="AG24" s="51">
         <f t="shared" si="0"/>
-        <v>158</v>
+        <v>378</v>
       </c>
       <c r="AH24">
         <v>128</v>
@@ -3748,12 +3762,14 @@
         <v>187</v>
       </c>
       <c r="AJ24" s="56" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="AK24" s="56">
         <v>30</v>
       </c>
-      <c r="AL24" s="93"/>
+      <c r="AL24" s="93">
+        <v>220</v>
+      </c>
       <c r="AM24" s="56"/>
       <c r="AN24" s="56"/>
       <c r="AO24" s="56"/>
@@ -3770,11 +3786,11 @@
       <c r="AW24" s="107"/>
       <c r="AX24" s="56"/>
       <c r="AY24" s="56">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AZ24" s="56">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="BA24" s="56"/>
       <c r="BB24">
@@ -3850,10 +3866,12 @@
       <c r="AV25" s="56"/>
       <c r="AW25" s="56"/>
       <c r="AX25" s="56"/>
-      <c r="AY25" s="56"/>
+      <c r="AY25" s="56">
+        <v>2</v>
+      </c>
       <c r="AZ25" s="56">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BA25" s="56"/>
       <c r="BB25">

</xml_diff>

<commit_message>
Miercoles de comer con Mariana
</commit_message>
<xml_diff>
--- a/Finanzas/2_Mayo-Ago_2018.xlsx
+++ b/Finanzas/2_Mayo-Ago_2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prestamo\Desktop\Adrifelcha_Lab25\Finanzas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\afchavez\Desktop\Adrifelcha_Lab25\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="216">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -660,6 +660,18 @@
   </si>
   <si>
     <t>MAYO</t>
+  </si>
+  <si>
+    <t>Saurus Burgers</t>
+  </si>
+  <si>
+    <t>Cafés Oficina; Café Jaime</t>
+  </si>
+  <si>
+    <t>QUINCENA 1</t>
+  </si>
+  <si>
+    <t>Infografia</t>
   </si>
 </sst>
 </file>
@@ -1554,7 +1566,7 @@
   <dimension ref="A1:BH963"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1845,7 +1857,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>36489</v>
+        <v>36167</v>
       </c>
       <c r="Z4" s="47">
         <v>43222</v>
@@ -2015,7 +2027,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I501)))-(SUM((X11:X499)))</f>
-        <v>381</v>
+        <v>59</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -2099,7 +2111,7 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>-11807</v>
+        <v>-12129</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
@@ -4521,21 +4533,36 @@
       <c r="AA31" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="AB31" s="49"/>
+      <c r="AB31" s="49" t="s">
+        <v>214</v>
+      </c>
       <c r="AC31" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-292</v>
       </c>
       <c r="AD31" s="50"/>
-      <c r="AE31" s="50"/>
+      <c r="AE31" s="50">
+        <v>20</v>
+      </c>
       <c r="AG31" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI31" s="106"/>
-      <c r="AJ31" s="56"/>
-      <c r="AK31" s="56"/>
-      <c r="AL31" s="56"/>
+        <v>312</v>
+      </c>
+      <c r="AH31">
+        <v>130</v>
+      </c>
+      <c r="AI31" s="106" t="s">
+        <v>212</v>
+      </c>
+      <c r="AJ31" s="56" t="s">
+        <v>213</v>
+      </c>
+      <c r="AK31" s="56">
+        <v>75</v>
+      </c>
+      <c r="AL31" s="56">
+        <v>107</v>
+      </c>
       <c r="AM31" s="56"/>
       <c r="AN31" s="56"/>
       <c r="AO31" s="56"/>
@@ -4600,21 +4627,29 @@
       <c r="AA32" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="AB32" s="49"/>
+      <c r="AB32" s="49" t="s">
+        <v>215</v>
+      </c>
       <c r="AC32" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-30</v>
       </c>
       <c r="AD32" s="50"/>
       <c r="AE32" s="50"/>
       <c r="AG32" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AH32" s="71"/>
-      <c r="AI32" s="56"/>
+        <v>30</v>
+      </c>
+      <c r="AH32" s="71">
+        <v>0</v>
+      </c>
+      <c r="AI32" s="56" t="s">
+        <v>191</v>
+      </c>
       <c r="AJ32" s="56"/>
-      <c r="AK32" s="56"/>
+      <c r="AK32" s="56">
+        <v>30</v>
+      </c>
       <c r="AL32" s="56"/>
       <c r="AM32" s="56"/>
       <c r="AN32" s="56"/>

</xml_diff>

<commit_message>
Finanzas Comida JL y Ram
</commit_message>
<xml_diff>
--- a/Finanzas/2_Mayo-Ago_2018.xlsx
+++ b/Finanzas/2_Mayo-Ago_2018.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="220">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -672,6 +672,18 @@
   </si>
   <si>
     <t>Infografia</t>
+  </si>
+  <si>
+    <t>Ram - Antojitos</t>
+  </si>
+  <si>
+    <t>Puse la propina</t>
+  </si>
+  <si>
+    <t>Cafés JL y Ram</t>
+  </si>
+  <si>
+    <t>Capuchino y cacahuates; JUMEX en la mañana</t>
   </si>
 </sst>
 </file>
@@ -1565,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,7 +1655,7 @@
       <c r="E2" s="56"/>
       <c r="F2" s="111">
         <f>N3-D2</f>
-        <v>4613</v>
+        <v>4543</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>2</v>
@@ -1770,7 +1782,7 @@
       </c>
       <c r="N3" s="25">
         <f>(SUM(D2,(K11:K501)))-(SUM((J11:J501),(I11:I501)))</f>
-        <v>12376</v>
+        <v>12306</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
@@ -1857,7 +1869,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>36167</v>
+        <v>36212</v>
       </c>
       <c r="Z4" s="47">
         <v>43222</v>
@@ -2027,7 +2039,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I501)))-(SUM((X11:X499)))</f>
-        <v>59</v>
+        <v>174</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -2111,7 +2123,7 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>-12129</v>
+        <v>-12014</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
@@ -3455,10 +3467,16 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G20" s="97"/>
-      <c r="H20" s="56"/>
+      <c r="G20" s="97">
+        <v>43251</v>
+      </c>
+      <c r="H20" s="56" t="s">
+        <v>218</v>
+      </c>
       <c r="I20" s="99"/>
-      <c r="J20" s="100"/>
+      <c r="J20" s="100">
+        <v>70</v>
+      </c>
       <c r="K20" s="101"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18" t="s">
@@ -4715,22 +4733,39 @@
       <c r="AA33" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="AB33" s="49"/>
+      <c r="AB33" s="49" t="s">
+        <v>216</v>
+      </c>
       <c r="AC33" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD33" s="50"/>
+        <v>115</v>
+      </c>
+      <c r="AD33" s="50">
+        <v>200</v>
+      </c>
       <c r="AE33" s="50"/>
       <c r="AG33" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI33" s="56"/>
-      <c r="AJ33" s="56"/>
-      <c r="AK33" s="106"/>
-      <c r="AL33" s="56"/>
-      <c r="AM33" s="56"/>
+        <v>85</v>
+      </c>
+      <c r="AH33">
+        <v>30</v>
+      </c>
+      <c r="AI33" s="56" t="s">
+        <v>217</v>
+      </c>
+      <c r="AJ33" s="56" t="s">
+        <v>219</v>
+      </c>
+      <c r="AK33" s="106">
+        <v>30</v>
+      </c>
+      <c r="AL33" s="56">
+        <v>5</v>
+      </c>
+      <c r="AM33" s="56">
+        <v>20</v>
+      </c>
       <c r="AN33" s="56"/>
       <c r="AO33" s="56"/>
       <c r="AP33" s="56"/>

</xml_diff>

<commit_message>
Gastos jueves con ale
</commit_message>
<xml_diff>
--- a/Finanzas/2_Mayo-Ago_2018.xlsx
+++ b/Finanzas/2_Mayo-Ago_2018.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="223">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -684,6 +684,15 @@
   </si>
   <si>
     <t>Capuchino y cacahuates; JUMEX en la mañana</t>
+  </si>
+  <si>
+    <t>Toks Ale</t>
+  </si>
+  <si>
+    <t>Ale</t>
+  </si>
+  <si>
+    <t>Concierto Harry</t>
   </si>
 </sst>
 </file>
@@ -1577,8 +1586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,7 +1664,7 @@
       <c r="E2" s="56"/>
       <c r="F2" s="111">
         <f>N3-D2</f>
-        <v>4543</v>
+        <v>4265</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>2</v>
@@ -1782,7 +1791,7 @@
       </c>
       <c r="N3" s="25">
         <f>(SUM(D2,(K11:K501)))-(SUM((J11:J501),(I11:I501)))</f>
-        <v>12306</v>
+        <v>12028</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
@@ -1869,7 +1878,7 @@
       </c>
       <c r="P4" s="79">
         <f>SUM(N3,R9,P7)</f>
-        <v>36212</v>
+        <v>36004</v>
       </c>
       <c r="Z4" s="47">
         <v>43222</v>
@@ -2039,7 +2048,7 @@
       </c>
       <c r="N6" s="52">
         <f>(SUM((W11:W299),(AC3:AC500),(I11:I501)))-(SUM((X11:X499)))</f>
-        <v>174</v>
+        <v>244</v>
       </c>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
@@ -2123,7 +2132,7 @@
       </c>
       <c r="P7" s="78">
         <f>SUM(R7,N6)</f>
-        <v>-12014</v>
+        <v>-11944</v>
       </c>
       <c r="Q7" s="75"/>
       <c r="R7" s="74">
@@ -3564,10 +3573,16 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G21" s="97"/>
-      <c r="H21" s="56"/>
+      <c r="G21" s="97">
+        <v>43251</v>
+      </c>
+      <c r="H21" s="56" t="s">
+        <v>220</v>
+      </c>
       <c r="I21" s="99"/>
-      <c r="J21" s="100"/>
+      <c r="J21" s="100">
+        <v>278</v>
+      </c>
       <c r="K21" s="101"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18" t="s">
@@ -4738,12 +4753,17 @@
       </c>
       <c r="AC33" s="41">
         <f t="shared" si="3"/>
-        <v>115</v>
+        <v>215</v>
       </c>
       <c r="AD33" s="50">
         <v>200</v>
       </c>
-      <c r="AE33" s="50"/>
+      <c r="AE33" s="50">
+        <v>100</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>221</v>
+      </c>
       <c r="AG33" s="51">
         <f t="shared" si="0"/>
         <v>85</v>
@@ -4829,20 +4849,24 @@
       <c r="AA34" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="AB34" s="49"/>
+      <c r="AB34" s="49" t="s">
+        <v>222</v>
+      </c>
       <c r="AC34" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-30</v>
       </c>
       <c r="AD34" s="50"/>
       <c r="AE34" s="50"/>
       <c r="AG34" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AI34" s="56"/>
       <c r="AJ34" s="56"/>
-      <c r="AK34" s="56"/>
+      <c r="AK34" s="56">
+        <v>30</v>
+      </c>
       <c r="AL34" s="56"/>
       <c r="AM34" s="56"/>
       <c r="AN34" s="56"/>

</xml_diff>

<commit_message>
Comida con Oli, Jorge y Oscar
</commit_message>
<xml_diff>
--- a/Finanzas/2_Mayo-Ago_2018.xlsx
+++ b/Finanzas/2_Mayo-Ago_2018.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="251">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -750,6 +750,33 @@
   </si>
   <si>
     <t>JL apoyo en revision de AFC</t>
+  </si>
+  <si>
+    <t>Capuchino y canasta de nata pa Cesar</t>
+  </si>
+  <si>
+    <t>Comida Jaime Clunys</t>
+  </si>
+  <si>
+    <t>Tarjeta Jaime</t>
+  </si>
+  <si>
+    <t>Capacitacion llenado de actas</t>
+  </si>
+  <si>
+    <t>Clunys</t>
+  </si>
+  <si>
+    <t>Clunys (Pago con tarjeta)</t>
+  </si>
+  <si>
+    <t>Reyes - Muro</t>
+  </si>
+  <si>
+    <t>Comida Oli, Jorge y Oscar</t>
+  </si>
+  <si>
+    <t>Tostadas</t>
   </si>
 </sst>
 </file>
@@ -1652,8 +1679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI963"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W29" workbookViewId="0">
-      <selection activeCell="AC41" sqref="AC41"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AD44" sqref="AD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1733,7 +1760,7 @@
       <c r="E2" s="55"/>
       <c r="F2" s="109">
         <f>N3-D2</f>
-        <v>806</v>
+        <v>-250</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>2</v>
@@ -1861,7 +1888,7 @@
       </c>
       <c r="N3" s="24">
         <f>(SUM(D2,(K11:K501)))-(SUM((J11:J501),(I11:I501)))</f>
-        <v>8569</v>
+        <v>7513</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
@@ -1949,7 +1976,7 @@
       </c>
       <c r="P4" s="78">
         <f>SUM(N3,S9,P7)</f>
-        <v>46597</v>
+        <v>45384</v>
       </c>
       <c r="Q4" s="55"/>
       <c r="AA4" s="46">
@@ -2018,7 +2045,7 @@
       </c>
       <c r="BH4" s="56">
         <f>(SUM((AW3:AW519)))-(SUM((BA3:BA519)))</f>
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="BI4" s="56"/>
     </row>
@@ -2120,7 +2147,7 @@
       </c>
       <c r="N6" s="51">
         <f>(SUM((X11:X299),(AD3:AD500),(I11:I501)))-(SUM((Y11:Y499)))</f>
-        <v>828</v>
+        <v>671</v>
       </c>
       <c r="O6" s="29"/>
       <c r="P6" s="29"/>
@@ -2204,7 +2231,7 @@
       </c>
       <c r="P7" s="77">
         <f>SUM(R7,N6)</f>
-        <v>828</v>
+        <v>671</v>
       </c>
       <c r="Q7" s="74"/>
       <c r="R7" s="73">
@@ -3509,7 +3536,7 @@
       </c>
       <c r="L19" s="134">
         <f>K19-N3</f>
-        <v>3619</v>
+        <v>4675</v>
       </c>
       <c r="M19" s="17"/>
       <c r="N19" s="17" t="s">
@@ -4196,10 +4223,16 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G26" s="95"/>
-      <c r="H26" s="55"/>
+      <c r="G26" s="95">
+        <v>43259</v>
+      </c>
+      <c r="H26" s="55" t="s">
+        <v>243</v>
+      </c>
       <c r="I26" s="97"/>
-      <c r="J26" s="98"/>
+      <c r="J26" s="98">
+        <v>1056</v>
+      </c>
       <c r="K26" s="99"/>
       <c r="M26" s="17"/>
       <c r="N26" s="17" t="s">
@@ -5603,7 +5636,9 @@
       <c r="AI40">
         <v>50</v>
       </c>
-      <c r="AJ40" s="55"/>
+      <c r="AJ40" s="55" t="s">
+        <v>187</v>
+      </c>
       <c r="AK40" s="55" t="s">
         <v>153</v>
       </c>
@@ -5668,21 +5703,34 @@
       <c r="AB41" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="AC41" s="48"/>
+      <c r="AC41" s="48" t="s">
+        <v>246</v>
+      </c>
       <c r="AD41" s="40">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-52</v>
       </c>
       <c r="AE41" s="49"/>
       <c r="AF41" s="106"/>
       <c r="AH41" s="50">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AJ41" s="55"/>
-      <c r="AK41" s="55"/>
-      <c r="AL41" s="55"/>
-      <c r="AM41" s="55"/>
+        <v>52</v>
+      </c>
+      <c r="AI41">
+        <v>0</v>
+      </c>
+      <c r="AJ41" s="55" t="s">
+        <v>247</v>
+      </c>
+      <c r="AK41" s="55" t="s">
+        <v>242</v>
+      </c>
+      <c r="AL41" s="55">
+        <v>30</v>
+      </c>
+      <c r="AM41" s="55">
+        <v>22</v>
+      </c>
       <c r="AN41" s="55"/>
       <c r="AO41" s="55"/>
       <c r="AP41" s="55"/>
@@ -5740,20 +5788,29 @@
       <c r="AB42" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="AC42" s="48"/>
+      <c r="AC42" s="48" t="s">
+        <v>245</v>
+      </c>
       <c r="AD42" s="40">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="AE42" s="49"/>
       <c r="AF42" s="49"/>
       <c r="AH42" s="50">
         <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="AI42">
         <v>0</v>
       </c>
       <c r="AJ42" s="55"/>
-      <c r="AK42" s="55"/>
-      <c r="AL42" s="55"/>
+      <c r="AK42" s="55" t="s">
+        <v>244</v>
+      </c>
+      <c r="AL42" s="55">
+        <v>20</v>
+      </c>
       <c r="AM42" s="55"/>
       <c r="AN42" s="55"/>
       <c r="AO42" s="55"/>
@@ -5770,10 +5827,12 @@
       <c r="AW42" s="55"/>
       <c r="AX42" s="55"/>
       <c r="AY42" s="55"/>
-      <c r="AZ42" s="55"/>
+      <c r="AZ42" s="55">
+        <v>5</v>
+      </c>
       <c r="BA42" s="55">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="BB42" s="55"/>
       <c r="BC42">
@@ -5812,7 +5871,9 @@
       <c r="AB43" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="AC43" s="48"/>
+      <c r="AC43" s="48" t="s">
+        <v>248</v>
+      </c>
       <c r="AD43" s="40">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -5821,6 +5882,9 @@
       <c r="AF43" s="49"/>
       <c r="AH43" s="50">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AI43">
         <v>0</v>
       </c>
       <c r="AJ43" s="55"/>
@@ -5884,20 +5948,31 @@
       <c r="AB44" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="AC44" s="71"/>
+      <c r="AC44" s="71" t="s">
+        <v>249</v>
+      </c>
       <c r="AD44" s="40">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-85</v>
       </c>
       <c r="AE44" s="49"/>
       <c r="AF44" s="49"/>
       <c r="AH44" s="50">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AJ44" s="96"/>
-      <c r="AK44" s="55"/>
-      <c r="AL44" s="55"/>
+        <v>85</v>
+      </c>
+      <c r="AI44">
+        <v>55</v>
+      </c>
+      <c r="AJ44" s="96" t="s">
+        <v>250</v>
+      </c>
+      <c r="AK44" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="AL44" s="55">
+        <v>30</v>
+      </c>
       <c r="AM44" s="55"/>
       <c r="AN44" s="55"/>
       <c r="AO44" s="55"/>

</xml_diff>

<commit_message>
Actualizando curso de estadística
</commit_message>
<xml_diff>
--- a/Finanzas/2_Mayo-Ago_2018.xlsx
+++ b/Finanzas/2_Mayo-Ago_2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="458">
   <si>
     <t>E L             D I N E R O         E  S             U N             R E C U R S O      L I M I T A D O</t>
   </si>
@@ -1330,6 +1330,75 @@
   </si>
   <si>
     <t>Faltan</t>
+  </si>
+  <si>
+    <t>Pizzas Rústicas</t>
+  </si>
+  <si>
+    <t>Papá cooperó</t>
+  </si>
+  <si>
+    <t>Comida Corrida CENEVAL</t>
+  </si>
+  <si>
+    <t>Gastos Quincena</t>
+  </si>
+  <si>
+    <t>CENEVAL 1</t>
+  </si>
+  <si>
+    <t>No llego Etapa 1</t>
+  </si>
+  <si>
+    <t>Pedro en Casa!</t>
+  </si>
+  <si>
+    <t>Jaime Afro Samurai</t>
+  </si>
+  <si>
+    <t>Pizza Rústica</t>
+  </si>
+  <si>
+    <t>Turnitin + Diada Uli-Pao</t>
+  </si>
+  <si>
+    <t>Obra Juancho</t>
+  </si>
+  <si>
+    <t>Torta + Refresco + Golosinas</t>
+  </si>
+  <si>
+    <t>Comida Corrida CENEVAL + Capuchino</t>
+  </si>
+  <si>
+    <t>Ale Primer día | Ceneval Pao y Daf</t>
+  </si>
+  <si>
+    <t>Alitas con Jaime</t>
+  </si>
+  <si>
+    <t>Uber a casa</t>
+  </si>
+  <si>
+    <t>Comida Corrida Esquina + Cheetos + Duvalin</t>
+  </si>
+  <si>
+    <t>Toks Nadia</t>
+  </si>
+  <si>
+    <t>Gasto 2 semanas</t>
+  </si>
+  <si>
+    <t>Propina Oscar + Patrick</t>
+  </si>
+  <si>
+    <t>Capuchino + Torta Jaime</t>
+  </si>
+  <si>
+    <t>Pizzas con Ale</t>
+  </si>
+  <si>
+    <t>Uber Pizzas con Ale</t>
   </si>
 </sst>
 </file>
@@ -2271,8 +2340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI963"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2356,7 +2425,7 @@
       <c r="E2" s="54"/>
       <c r="F2" s="107">
         <f>N3-D2</f>
-        <v>9122.7900000000009</v>
+        <v>13701.79</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>2</v>
@@ -2484,7 +2553,7 @@
       </c>
       <c r="N3" s="23">
         <f>(SUM(D2,(K11:K503)))-(SUM((J11:J503),(I11:I503)))</f>
-        <v>16885.79</v>
+        <v>21464.79</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
@@ -2572,7 +2641,7 @@
       </c>
       <c r="P4" s="76">
         <f>SUM(N3,S9,P7)</f>
-        <v>77777.790000000008</v>
+        <v>86688.290000000008</v>
       </c>
       <c r="Q4" s="54"/>
       <c r="AA4" s="45">
@@ -2641,7 +2710,7 @@
       </c>
       <c r="BH4" s="55">
         <f>(SUM((AW3:AW519)))-(SUM((BA3:BA519)))</f>
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="BI4" s="55"/>
     </row>
@@ -2743,7 +2812,7 @@
       </c>
       <c r="N6" s="50">
         <f>(SUM((X11:X299),(AD3:AD500),(I11:I503)))-(SUM((Y11:Y499)))</f>
-        <v>-129</v>
+        <v>303.5</v>
       </c>
       <c r="O6" s="28"/>
       <c r="P6" s="28"/>
@@ -2827,12 +2896,12 @@
       </c>
       <c r="P7" s="75">
         <f>SUM(R7,N6)</f>
-        <v>-128</v>
+        <v>303.5</v>
       </c>
       <c r="Q7" s="72"/>
       <c r="R7" s="71">
         <f>(SUM(Y11:Y499))-(SUM(K11:K503))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7" s="109"/>
       <c r="T7" s="111">
@@ -2989,8 +3058,8 @@
         <v>25</v>
       </c>
       <c r="S9" s="13">
-        <f>SUM(S11:S491)</f>
-        <v>61020</v>
+        <f>SUM(S11:S492)</f>
+        <v>64920</v>
       </c>
       <c r="U9" s="30" t="s">
         <v>40</v>
@@ -3232,12 +3301,12 @@
       </c>
       <c r="R11" s="20"/>
       <c r="S11" s="18">
-        <f t="shared" ref="S11:S35" si="6">Q11-R11</f>
+        <f t="shared" ref="S11:S36" si="6">Q11-R11</f>
         <v>5000</v>
       </c>
       <c r="T11" s="125">
-        <f>SUM(S11:S23)</f>
-        <v>46350</v>
+        <f>SUM(S11:S24)</f>
+        <v>50250</v>
       </c>
       <c r="U11" s="34">
         <v>43221</v>
@@ -3482,7 +3551,7 @@
       </c>
       <c r="R13" s="20"/>
       <c r="S13" s="18">
-        <f t="shared" ref="S13:S23" si="7">Q13-R13</f>
+        <f t="shared" ref="S13:S24" si="7">Q13-R13</f>
         <v>3200</v>
       </c>
       <c r="T13" s="124"/>
@@ -4731,25 +4800,23 @@
       </c>
       <c r="J24" s="96"/>
       <c r="K24" s="97"/>
-      <c r="M24" s="16"/>
+      <c r="M24" s="57">
+        <v>43331</v>
+      </c>
       <c r="N24" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O24" s="16" t="s">
-        <v>34</v>
+        <v>453</v>
       </c>
       <c r="P24" s="33"/>
       <c r="Q24" s="21">
-        <v>1100</v>
+        <v>3900</v>
       </c>
       <c r="R24" s="20"/>
       <c r="S24" s="18">
-        <f t="shared" si="6"/>
-        <v>1100</v>
-      </c>
-      <c r="T24" s="124">
-        <f>SUM(S24:S35)</f>
-        <v>5270</v>
+        <f t="shared" si="7"/>
+        <v>3900</v>
       </c>
       <c r="U24" s="34">
         <v>43293</v>
@@ -4849,18 +4916,21 @@
         <v>24</v>
       </c>
       <c r="O25" s="16" t="s">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="P25" s="33"/>
       <c r="Q25" s="21">
-        <v>600</v>
+        <v>1100</v>
       </c>
       <c r="R25" s="20"/>
       <c r="S25" s="18">
         <f t="shared" si="6"/>
-        <v>600</v>
-      </c>
-      <c r="T25" s="124"/>
+        <v>1100</v>
+      </c>
+      <c r="T25" s="124">
+        <f>SUM(S25:S36)</f>
+        <v>5270</v>
+      </c>
       <c r="U25" s="142">
         <v>43295</v>
       </c>
@@ -4953,16 +5023,16 @@
         <v>24</v>
       </c>
       <c r="O26" s="16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P26" s="33"/>
       <c r="Q26" s="21">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="R26" s="20"/>
       <c r="S26" s="18">
-        <f>Q26-R26</f>
-        <v>1000</v>
+        <f t="shared" si="6"/>
+        <v>600</v>
       </c>
       <c r="T26" s="124"/>
       <c r="U26" s="34">
@@ -4973,10 +5043,10 @@
       </c>
       <c r="W26" s="33"/>
       <c r="X26" s="35">
-        <v>11052</v>
+        <v>11051</v>
       </c>
       <c r="Y26" s="35">
-        <v>11052</v>
+        <v>11051</v>
       </c>
       <c r="AA26" s="45">
         <v>43244</v>
@@ -5070,16 +5140,16 @@
         <v>24</v>
       </c>
       <c r="O27" s="16" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="P27" s="33"/>
       <c r="Q27" s="21">
-        <v>120</v>
+        <v>1000</v>
       </c>
       <c r="R27" s="20"/>
       <c r="S27" s="18">
-        <f t="shared" si="6"/>
-        <v>120</v>
+        <f>Q27-R27</f>
+        <v>1000</v>
       </c>
       <c r="T27" s="124"/>
       <c r="U27" s="34">
@@ -5187,16 +5257,16 @@
         <v>24</v>
       </c>
       <c r="O28" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P28" s="33"/>
       <c r="Q28" s="21">
-        <v>500</v>
+        <v>120</v>
       </c>
       <c r="R28" s="20"/>
       <c r="S28" s="18">
         <f t="shared" si="6"/>
-        <v>500</v>
+        <v>120</v>
       </c>
       <c r="T28" s="124"/>
       <c r="U28" s="34">
@@ -5295,23 +5365,31 @@
         <v>24</v>
       </c>
       <c r="O29" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P29" s="33"/>
       <c r="Q29" s="21">
-        <v>150</v>
+        <v>500</v>
       </c>
       <c r="R29" s="20"/>
       <c r="S29" s="18">
         <f t="shared" si="6"/>
-        <v>150</v>
+        <v>500</v>
       </c>
       <c r="T29" s="124"/>
-      <c r="U29" s="34"/>
-      <c r="V29" s="33"/>
+      <c r="U29" s="34">
+        <v>43326</v>
+      </c>
+      <c r="V29" s="33" t="s">
+        <v>205</v>
+      </c>
       <c r="W29" s="33"/>
-      <c r="X29" s="35"/>
-      <c r="Y29" s="35"/>
+      <c r="X29" s="35">
+        <v>11052</v>
+      </c>
+      <c r="Y29" s="35">
+        <v>11052</v>
+      </c>
       <c r="AA29" s="45">
         <v>43247</v>
       </c>
@@ -5391,17 +5469,18 @@
         <v>24</v>
       </c>
       <c r="O30" s="16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P30" s="33"/>
       <c r="Q30" s="21">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="R30" s="20"/>
       <c r="S30" s="18">
         <f t="shared" si="6"/>
-        <v>100</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="T30" s="124"/>
       <c r="U30" s="34"/>
       <c r="V30" s="33"/>
       <c r="W30" s="33"/>
@@ -5496,18 +5575,17 @@
         <v>24</v>
       </c>
       <c r="O31" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P31" s="33"/>
       <c r="Q31" s="21">
-        <v>850</v>
+        <v>100</v>
       </c>
       <c r="R31" s="20"/>
       <c r="S31" s="18">
         <f t="shared" si="6"/>
-        <v>850</v>
-      </c>
-      <c r="T31" s="124"/>
+        <v>100</v>
+      </c>
       <c r="U31" s="34"/>
       <c r="V31" s="33"/>
       <c r="W31" s="33"/>
@@ -5598,16 +5676,16 @@
         <v>24</v>
       </c>
       <c r="O32" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P32" s="33"/>
       <c r="Q32" s="21">
-        <v>300</v>
+        <v>850</v>
       </c>
       <c r="R32" s="20"/>
       <c r="S32" s="18">
         <f t="shared" si="6"/>
-        <v>300</v>
+        <v>850</v>
       </c>
       <c r="T32" s="124"/>
       <c r="U32" s="34"/>
@@ -5694,16 +5772,16 @@
         <v>24</v>
       </c>
       <c r="O33" s="16" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="P33" s="33"/>
       <c r="Q33" s="21">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="R33" s="20"/>
       <c r="S33" s="18">
         <f t="shared" si="6"/>
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="T33" s="124"/>
       <c r="U33" s="34"/>
@@ -5803,16 +5881,16 @@
         <v>24</v>
       </c>
       <c r="O34" s="16" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="P34" s="33"/>
       <c r="Q34" s="21">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="R34" s="20"/>
       <c r="S34" s="18">
         <f t="shared" si="6"/>
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="T34" s="124"/>
       <c r="U34" s="34"/>
@@ -5905,17 +5983,18 @@
         <v>24</v>
       </c>
       <c r="O35" s="16" t="s">
-        <v>383</v>
+        <v>65</v>
       </c>
       <c r="P35" s="33"/>
       <c r="Q35" s="21">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="R35" s="20"/>
       <c r="S35" s="18">
         <f t="shared" si="6"/>
-        <v>150</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="T35" s="124"/>
       <c r="U35" s="34"/>
       <c r="V35" s="33"/>
       <c r="W35" s="33"/>
@@ -5997,27 +6076,21 @@
         <v>413</v>
       </c>
       <c r="K36" s="97"/>
-      <c r="M36" s="57">
-        <v>42802</v>
-      </c>
+      <c r="M36" s="16"/>
       <c r="N36" s="16" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="O36" s="16" t="s">
-        <v>63</v>
+        <v>383</v>
       </c>
       <c r="P36" s="33"/>
       <c r="Q36" s="21">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="R36" s="20"/>
       <c r="S36" s="18">
-        <f>Q36-R36</f>
-        <v>140</v>
-      </c>
-      <c r="T36" s="124">
-        <f>SUM(S36:S37)</f>
-        <v>340</v>
+        <f t="shared" si="6"/>
+        <v>150</v>
       </c>
       <c r="U36" s="34"/>
       <c r="V36" s="33"/>
@@ -6099,16 +6172,20 @@
         <v>62</v>
       </c>
       <c r="O37" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P37" s="33"/>
       <c r="Q37" s="21">
-        <v>200</v>
+        <v>140</v>
       </c>
       <c r="R37" s="20"/>
       <c r="S37" s="18">
         <f>Q37-R37</f>
-        <v>200</v>
+        <v>140</v>
+      </c>
+      <c r="T37" s="124">
+        <f>SUM(S37:S38)</f>
+        <v>340</v>
       </c>
       <c r="U37" s="34"/>
       <c r="V37" s="33"/>
@@ -6194,22 +6271,22 @@
       <c r="J38" s="96"/>
       <c r="K38" s="97"/>
       <c r="M38" s="57">
-        <v>43266</v>
+        <v>42802</v>
       </c>
       <c r="N38" s="16" t="s">
         <v>62</v>
       </c>
       <c r="O38" s="16" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="P38" s="33"/>
       <c r="Q38" s="21">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="R38" s="20"/>
       <c r="S38" s="18">
         <f>Q38-R38</f>
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="U38" s="34"/>
       <c r="V38" s="33"/>
@@ -6296,23 +6373,23 @@
       </c>
       <c r="J39" s="96"/>
       <c r="K39" s="97"/>
-      <c r="M39" s="16"/>
+      <c r="M39" s="57">
+        <v>43266</v>
+      </c>
       <c r="N39" s="16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O39" s="16" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="P39" s="33"/>
       <c r="Q39" s="21">
-        <v>1800</v>
-      </c>
-      <c r="R39" s="20">
-        <v>1150</v>
-      </c>
+        <v>5000</v>
+      </c>
+      <c r="R39" s="20"/>
       <c r="S39" s="18">
         <f>Q39-R39</f>
-        <v>650</v>
+        <v>5000</v>
       </c>
       <c r="U39" s="34"/>
       <c r="V39" s="33"/>
@@ -6397,23 +6474,23 @@
         <v>497</v>
       </c>
       <c r="K40" s="97"/>
-      <c r="M40" s="57">
-        <v>43010</v>
-      </c>
+      <c r="M40" s="16"/>
       <c r="N40" s="16" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="O40" s="16" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="P40" s="33"/>
       <c r="Q40" s="21">
-        <v>100</v>
-      </c>
-      <c r="R40" s="20"/>
+        <v>1800</v>
+      </c>
+      <c r="R40" s="20">
+        <v>1150</v>
+      </c>
       <c r="S40" s="18">
-        <f t="shared" ref="S40:S74" si="9">Q40-R40</f>
-        <v>100</v>
+        <f>Q40-R40</f>
+        <v>650</v>
       </c>
       <c r="U40" s="34"/>
       <c r="V40" s="33"/>
@@ -6498,31 +6575,23 @@
         <v>244</v>
       </c>
       <c r="K41" s="97"/>
-      <c r="M41" s="16" t="s">
-        <v>97</v>
+      <c r="M41" s="57">
+        <v>43010</v>
       </c>
       <c r="N41" s="16" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
       <c r="O41" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="P41" s="33" t="s">
-        <v>347</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="P41" s="33"/>
       <c r="Q41" s="21">
-        <v>1040</v>
-      </c>
-      <c r="R41" s="20">
-        <v>500</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="R41" s="20"/>
       <c r="S41" s="18">
-        <f t="shared" si="9"/>
-        <v>540</v>
-      </c>
-      <c r="T41" s="124">
-        <f>SUM(S41:S48)</f>
-        <v>3110</v>
+        <f t="shared" ref="S41:S75" si="9">Q41-R41</f>
+        <v>100</v>
       </c>
       <c r="U41" s="34"/>
       <c r="V41" s="33"/>
@@ -6609,23 +6678,31 @@
         <v>30</v>
       </c>
       <c r="K42" s="97"/>
-      <c r="M42" s="16"/>
+      <c r="M42" s="16" t="s">
+        <v>97</v>
+      </c>
       <c r="N42" s="16" t="s">
         <v>26</v>
       </c>
       <c r="O42" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="P42" s="33"/>
+        <v>96</v>
+      </c>
+      <c r="P42" s="33" t="s">
+        <v>347</v>
+      </c>
       <c r="Q42" s="21">
-        <v>2900</v>
+        <v>1040</v>
       </c>
       <c r="R42" s="20">
-        <v>1550</v>
+        <v>500</v>
       </c>
       <c r="S42" s="18">
         <f t="shared" si="9"/>
-        <v>1350</v>
+        <v>540</v>
+      </c>
+      <c r="T42" s="124">
+        <f>SUM(S42:S49)</f>
+        <v>3110</v>
       </c>
       <c r="U42" s="34"/>
       <c r="V42" s="33"/>
@@ -6711,16 +6788,18 @@
         <v>26</v>
       </c>
       <c r="O43" s="16" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="P43" s="33"/>
       <c r="Q43" s="21">
-        <v>240</v>
-      </c>
-      <c r="R43" s="20"/>
+        <v>2900</v>
+      </c>
+      <c r="R43" s="20">
+        <v>1550</v>
+      </c>
       <c r="S43" s="18">
         <f t="shared" si="9"/>
-        <v>240</v>
+        <v>1350</v>
       </c>
       <c r="U43" s="34"/>
       <c r="V43" s="33"/>
@@ -6795,27 +6874,21 @@
       <c r="K44" s="140">
         <v>1317</v>
       </c>
-      <c r="M44" s="16" t="s">
-        <v>120</v>
-      </c>
+      <c r="M44" s="16"/>
       <c r="N44" s="16" t="s">
         <v>26</v>
       </c>
       <c r="O44" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="P44" s="33" t="s">
-        <v>232</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="P44" s="33"/>
       <c r="Q44" s="21">
-        <v>1500</v>
-      </c>
-      <c r="R44" s="20">
-        <v>1300</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="R44" s="20"/>
       <c r="S44" s="18">
-        <f>Q44-R44</f>
-        <v>200</v>
+        <f t="shared" si="9"/>
+        <v>240</v>
       </c>
       <c r="U44" s="34"/>
       <c r="V44" s="33"/>
@@ -6833,11 +6906,11 @@
       </c>
       <c r="AD44" s="39">
         <f t="shared" si="3"/>
-        <v>173</v>
+        <v>297</v>
       </c>
       <c r="AE44" s="48"/>
       <c r="AF44" s="132">
-        <v>308</v>
+        <v>432</v>
       </c>
       <c r="AG44" t="s">
         <v>274</v>
@@ -6903,21 +6976,27 @@
         <v>310</v>
       </c>
       <c r="K45" s="97"/>
-      <c r="M45" s="16"/>
+      <c r="M45" s="16" t="s">
+        <v>120</v>
+      </c>
       <c r="N45" s="16" t="s">
         <v>26</v>
       </c>
       <c r="O45" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="P45" s="33"/>
+        <v>121</v>
+      </c>
+      <c r="P45" s="33" t="s">
+        <v>232</v>
+      </c>
       <c r="Q45" s="21">
-        <v>100</v>
-      </c>
-      <c r="R45" s="20"/>
+        <v>1500</v>
+      </c>
+      <c r="R45" s="20">
+        <v>1300</v>
+      </c>
       <c r="S45" s="18">
-        <f t="shared" si="9"/>
-        <v>100</v>
+        <f>Q45-R45</f>
+        <v>200</v>
       </c>
       <c r="U45" s="34"/>
       <c r="V45" s="33"/>
@@ -7006,16 +7085,16 @@
         <v>26</v>
       </c>
       <c r="O46" s="16" t="s">
-        <v>236</v>
+        <v>124</v>
       </c>
       <c r="P46" s="33"/>
       <c r="Q46" s="21">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="R46" s="20"/>
       <c r="S46" s="18">
         <f t="shared" si="9"/>
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="U46" s="34"/>
       <c r="V46" s="33"/>
@@ -7096,19 +7175,19 @@
       <c r="K47" s="97"/>
       <c r="M47" s="16"/>
       <c r="N47" s="16" t="s">
-        <v>233</v>
+        <v>26</v>
       </c>
       <c r="O47" s="16" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="P47" s="33"/>
       <c r="Q47" s="21">
-        <v>80</v>
+        <v>500</v>
       </c>
       <c r="R47" s="20"/>
       <c r="S47" s="18">
         <f t="shared" si="9"/>
-        <v>80</v>
+        <v>500</v>
       </c>
       <c r="U47" s="34"/>
       <c r="V47" s="33"/>
@@ -7193,19 +7272,19 @@
       <c r="K48" s="54"/>
       <c r="M48" s="16"/>
       <c r="N48" s="16" t="s">
-        <v>26</v>
+        <v>233</v>
       </c>
       <c r="O48" s="16" t="s">
-        <v>374</v>
+        <v>234</v>
       </c>
       <c r="P48" s="33"/>
       <c r="Q48" s="21">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="R48" s="20"/>
       <c r="S48" s="18">
         <f t="shared" si="9"/>
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="U48" s="34"/>
       <c r="V48" s="33"/>
@@ -7292,25 +7371,19 @@
       <c r="K49" s="97"/>
       <c r="M49" s="16"/>
       <c r="N49" s="16" t="s">
-        <v>122</v>
+        <v>26</v>
       </c>
       <c r="O49" s="16" t="s">
-        <v>123</v>
+        <v>374</v>
       </c>
       <c r="P49" s="33"/>
       <c r="Q49" s="21">
-        <v>130</v>
-      </c>
-      <c r="R49" s="20">
-        <v>130</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="R49" s="20"/>
       <c r="S49" s="18">
-        <f>Q49-R49</f>
-        <v>0</v>
-      </c>
-      <c r="T49" s="10">
-        <f>SUM(S49:S50)</f>
-        <v>200</v>
+        <f t="shared" si="9"/>
+        <v>100</v>
       </c>
       <c r="U49" s="34"/>
       <c r="V49" s="33"/>
@@ -7401,22 +7474,26 @@
       </c>
       <c r="J50" s="96"/>
       <c r="K50" s="97"/>
-      <c r="M50" s="57">
-        <v>43180</v>
-      </c>
+      <c r="M50" s="16"/>
       <c r="N50" s="16" t="s">
-        <v>253</v>
+        <v>122</v>
       </c>
       <c r="O50" s="16" t="s">
-        <v>254</v>
+        <v>123</v>
       </c>
       <c r="P50" s="33"/>
       <c r="Q50" s="21">
-        <v>200</v>
-      </c>
-      <c r="R50" s="20"/>
+        <v>130</v>
+      </c>
+      <c r="R50" s="20">
+        <v>130</v>
+      </c>
       <c r="S50" s="18">
-        <f t="shared" si="9"/>
+        <f>Q50-R50</f>
+        <v>0</v>
+      </c>
+      <c r="T50" s="10">
+        <f>SUM(S50:S51)</f>
         <v>200</v>
       </c>
       <c r="U50" s="34"/>
@@ -7490,24 +7567,22 @@
       </c>
       <c r="K51" s="97"/>
       <c r="M51" s="57">
-        <v>43266</v>
+        <v>43180</v>
       </c>
       <c r="N51" s="16" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="O51" s="16" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="P51" s="33"/>
       <c r="Q51" s="21">
-        <v>55</v>
-      </c>
-      <c r="R51" s="20">
-        <v>55</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="R51" s="20"/>
       <c r="S51" s="18">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="U51" s="34"/>
       <c r="V51" s="33"/>
@@ -7601,17 +7676,17 @@
         <v>43266</v>
       </c>
       <c r="N52" s="16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="O52" s="16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="P52" s="33"/>
       <c r="Q52" s="21">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="R52" s="20">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="S52" s="18">
         <f t="shared" si="9"/>
@@ -7704,12 +7779,22 @@
         <v>30</v>
       </c>
       <c r="K53" s="97"/>
-      <c r="M53" s="16"/>
-      <c r="N53" s="16"/>
-      <c r="O53" s="16"/>
+      <c r="M53" s="57">
+        <v>43266</v>
+      </c>
+      <c r="N53" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="O53" s="16" t="s">
+        <v>268</v>
+      </c>
       <c r="P53" s="33"/>
-      <c r="Q53" s="21"/>
-      <c r="R53" s="20"/>
+      <c r="Q53" s="21">
+        <v>60</v>
+      </c>
+      <c r="R53" s="20">
+        <v>60</v>
+      </c>
       <c r="S53" s="18">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -8584,6 +8669,15 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="G63" s="113">
+        <v>43322</v>
+      </c>
+      <c r="H63" t="s">
+        <v>435</v>
+      </c>
+      <c r="J63" s="10">
+        <v>231</v>
+      </c>
       <c r="K63" s="12"/>
       <c r="M63" s="16"/>
       <c r="N63" s="16"/>
@@ -8611,13 +8705,13 @@
       </c>
       <c r="AD63" s="39">
         <f t="shared" si="3"/>
-        <v>-5455</v>
+        <v>-5355</v>
       </c>
       <c r="AE63" s="48">
         <v>200</v>
       </c>
       <c r="AF63" s="48">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="AG63" t="s">
         <v>307</v>
@@ -8687,7 +8781,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K64" s="12"/>
+      <c r="G64" s="119">
+        <v>43326</v>
+      </c>
+      <c r="H64" s="120" t="s">
+        <v>205</v>
+      </c>
+      <c r="I64" s="131"/>
+      <c r="J64" s="122"/>
+      <c r="K64" s="123">
+        <v>11052</v>
+      </c>
       <c r="M64" s="16"/>
       <c r="N64" s="16"/>
       <c r="O64" s="16"/>
@@ -8757,6 +8861,15 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="G65" s="113">
+        <v>43326</v>
+      </c>
+      <c r="H65" t="s">
+        <v>207</v>
+      </c>
+      <c r="J65" s="10">
+        <v>202</v>
+      </c>
       <c r="K65" s="12"/>
       <c r="M65" s="16"/>
       <c r="N65" s="16"/>
@@ -8838,6 +8951,15 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="G66" s="113">
+        <v>43326</v>
+      </c>
+      <c r="H66" t="s">
+        <v>438</v>
+      </c>
+      <c r="I66" s="11">
+        <v>600</v>
+      </c>
       <c r="K66" s="12"/>
       <c r="M66" s="16"/>
       <c r="N66" s="16"/>
@@ -8919,6 +9041,15 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="G67" s="113">
+        <v>43326</v>
+      </c>
+      <c r="H67" t="s">
+        <v>445</v>
+      </c>
+      <c r="J67" s="10">
+        <v>80</v>
+      </c>
       <c r="K67" s="12"/>
       <c r="M67" s="16"/>
       <c r="N67" s="16"/>
@@ -9004,6 +9135,15 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="G68" s="113">
+        <v>43328</v>
+      </c>
+      <c r="H68" t="s">
+        <v>449</v>
+      </c>
+      <c r="J68" s="10">
+        <v>176</v>
+      </c>
       <c r="K68" s="12"/>
       <c r="M68" s="16"/>
       <c r="N68" s="16"/>
@@ -9085,6 +9225,15 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="G69" s="113">
+        <v>43328</v>
+      </c>
+      <c r="H69" t="s">
+        <v>450</v>
+      </c>
+      <c r="J69" s="10">
+        <v>204</v>
+      </c>
       <c r="K69" s="12"/>
       <c r="M69" s="16"/>
       <c r="N69" s="16"/>
@@ -9168,6 +9317,15 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="G70" s="113">
+        <v>43331</v>
+      </c>
+      <c r="H70" t="s">
+        <v>220</v>
+      </c>
+      <c r="I70" s="11">
+        <v>4000</v>
+      </c>
       <c r="K70" s="12"/>
       <c r="M70" s="16"/>
       <c r="N70" s="16"/>
@@ -9252,6 +9410,15 @@
       <c r="E71">
         <f t="shared" si="5"/>
         <v>0</v>
+      </c>
+      <c r="G71" s="113">
+        <v>43331</v>
+      </c>
+      <c r="H71" t="s">
+        <v>452</v>
+      </c>
+      <c r="J71" s="10">
+        <v>349</v>
       </c>
       <c r="K71" s="12"/>
       <c r="M71" s="16"/>
@@ -9333,6 +9500,15 @@
       <c r="E72">
         <f t="shared" si="5"/>
         <v>0</v>
+      </c>
+      <c r="G72" s="113">
+        <v>43333</v>
+      </c>
+      <c r="H72" t="s">
+        <v>456</v>
+      </c>
+      <c r="J72" s="10">
+        <v>440</v>
       </c>
       <c r="K72" s="12"/>
       <c r="M72" s="16"/>
@@ -9413,6 +9589,15 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="G73" s="113">
+        <v>43333</v>
+      </c>
+      <c r="H73" t="s">
+        <v>457</v>
+      </c>
+      <c r="J73" s="10">
+        <v>191</v>
+      </c>
       <c r="K73" s="12"/>
       <c r="M73" s="16"/>
       <c r="N73" s="16"/>
@@ -9584,7 +9769,7 @@
       <c r="Q75" s="21"/>
       <c r="R75" s="20"/>
       <c r="S75" s="18">
-        <f t="shared" ref="S75:S129" si="15">Q75-R75</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U75" s="33"/>
@@ -9663,7 +9848,7 @@
       <c r="Q76" s="21"/>
       <c r="R76" s="20"/>
       <c r="S76" s="18">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="S76:S130" si="15">Q76-R76</f>
         <v>0</v>
       </c>
       <c r="U76" s="33"/>
@@ -11767,10 +11952,12 @@
       </c>
       <c r="AX100" s="54"/>
       <c r="AY100" s="54"/>
-      <c r="AZ100" s="54"/>
+      <c r="AZ100" s="54">
+        <v>2</v>
+      </c>
       <c r="BA100" s="54">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BB100" s="54"/>
       <c r="BC100">
@@ -11855,10 +12042,12 @@
       <c r="AW101" s="54"/>
       <c r="AX101" s="54"/>
       <c r="AY101" s="54"/>
-      <c r="AZ101" s="54"/>
+      <c r="AZ101" s="54">
+        <v>2</v>
+      </c>
       <c r="BA101" s="54">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BB101" s="54"/>
       <c r="BC101">
@@ -11937,10 +12126,12 @@
       <c r="AW102" s="54"/>
       <c r="AX102" s="54"/>
       <c r="AY102" s="54"/>
-      <c r="AZ102" s="54"/>
+      <c r="AZ102" s="54">
+        <v>2</v>
+      </c>
       <c r="BA102" s="54">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BB102" s="54"/>
       <c r="BC102">
@@ -12019,10 +12210,12 @@
       <c r="AW103" s="54"/>
       <c r="AX103" s="54"/>
       <c r="AY103" s="54"/>
-      <c r="AZ103" s="54"/>
+      <c r="AZ103" s="54">
+        <v>2</v>
+      </c>
       <c r="BA103" s="54">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BB103" s="54"/>
       <c r="BC103">
@@ -12063,7 +12256,9 @@
       <c r="AB104" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="AC104" s="47"/>
+      <c r="AC104" s="47" t="s">
+        <v>443</v>
+      </c>
       <c r="AD104" s="39">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -12075,7 +12270,9 @@
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="AI104" s="54"/>
+      <c r="AI104" s="54" t="s">
+        <v>83</v>
+      </c>
       <c r="AJ104" s="54"/>
       <c r="AK104" s="54"/>
       <c r="AL104" s="54"/>
@@ -12095,10 +12292,12 @@
       <c r="AW104" s="54"/>
       <c r="AX104" s="54"/>
       <c r="AY104" s="54"/>
-      <c r="AZ104" s="54"/>
+      <c r="AZ104" s="54">
+        <v>2</v>
+      </c>
       <c r="BA104" s="54">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BB104" s="54"/>
       <c r="BC104">
@@ -12139,7 +12338,9 @@
       <c r="AB105" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="AC105" s="47"/>
+      <c r="AC105" s="47" t="s">
+        <v>442</v>
+      </c>
       <c r="AD105" s="39">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -12151,7 +12352,9 @@
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="AI105" s="54"/>
+      <c r="AI105" s="54" t="s">
+        <v>349</v>
+      </c>
       <c r="AJ105" s="54"/>
       <c r="AK105" s="54"/>
       <c r="AL105" s="54"/>
@@ -12215,7 +12418,9 @@
       <c r="AB106" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="AC106" s="47"/>
+      <c r="AC106" s="47" t="s">
+        <v>441</v>
+      </c>
       <c r="AD106" s="39">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -12291,20 +12496,30 @@
       <c r="AB107" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="AC107" s="47"/>
+      <c r="AC107" s="47" t="s">
+        <v>439</v>
+      </c>
       <c r="AD107" s="39">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AE107" s="48"/>
-      <c r="AF107" s="48"/>
-      <c r="AG107" s="54"/>
+      <c r="AF107" s="48">
+        <v>120</v>
+      </c>
+      <c r="AG107" s="54" t="s">
+        <v>436</v>
+      </c>
       <c r="AH107" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AI107" s="54"/>
-      <c r="AJ107" s="54"/>
+        <v>95</v>
+      </c>
+      <c r="AI107" s="54">
+        <v>45</v>
+      </c>
+      <c r="AJ107" s="54" t="s">
+        <v>437</v>
+      </c>
       <c r="AK107" s="54"/>
       <c r="AL107" s="54"/>
       <c r="AM107" s="54"/>
@@ -12318,15 +12533,21 @@
       <c r="AU107" s="54"/>
       <c r="AV107">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AW107" s="54"/>
-      <c r="AX107" s="54"/>
+        <v>50</v>
+      </c>
+      <c r="AW107" s="54">
+        <v>50</v>
+      </c>
+      <c r="AX107" s="54">
+        <v>1</v>
+      </c>
       <c r="AY107" s="54"/>
-      <c r="AZ107" s="54"/>
+      <c r="AZ107" s="54">
+        <v>2</v>
+      </c>
       <c r="BA107" s="54">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="BB107" s="54"/>
       <c r="BC107">
@@ -12367,22 +12588,30 @@
       <c r="AB108" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="AC108" s="47"/>
+      <c r="AC108" s="47" t="s">
+        <v>440</v>
+      </c>
       <c r="AD108" s="39">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-74</v>
       </c>
       <c r="AE108" s="48"/>
       <c r="AF108" s="48"/>
       <c r="AG108" s="54"/>
       <c r="AH108" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AI108" s="54"/>
-      <c r="AJ108" s="54"/>
+        <v>74</v>
+      </c>
+      <c r="AI108" s="54">
+        <v>63</v>
+      </c>
+      <c r="AJ108" s="54" t="s">
+        <v>446</v>
+      </c>
       <c r="AK108" s="54"/>
-      <c r="AL108" s="54"/>
+      <c r="AL108" s="54">
+        <v>11</v>
+      </c>
       <c r="AM108" s="54"/>
       <c r="AN108" s="54"/>
       <c r="AO108" s="54"/>
@@ -12397,12 +12626,16 @@
         <v>0</v>
       </c>
       <c r="AW108" s="54"/>
-      <c r="AX108" s="54"/>
+      <c r="AX108" s="54">
+        <v>1</v>
+      </c>
       <c r="AY108" s="54"/>
-      <c r="AZ108" s="54"/>
+      <c r="AZ108" s="54">
+        <v>1</v>
+      </c>
       <c r="BA108" s="54">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="BB108" s="54"/>
       <c r="BC108">
@@ -12443,22 +12676,30 @@
       <c r="AB109" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="AC109" s="47"/>
+      <c r="AC109" s="47" t="s">
+        <v>444</v>
+      </c>
       <c r="AD109" s="39">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-82.5</v>
       </c>
       <c r="AE109" s="48"/>
       <c r="AF109" s="48"/>
       <c r="AG109" s="54"/>
       <c r="AH109" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AI109" s="54"/>
-      <c r="AJ109" s="54"/>
+        <v>82.5</v>
+      </c>
+      <c r="AI109" s="54">
+        <v>45</v>
+      </c>
+      <c r="AJ109" s="54" t="s">
+        <v>447</v>
+      </c>
       <c r="AK109" s="54"/>
-      <c r="AL109" s="54"/>
+      <c r="AL109" s="54">
+        <v>30</v>
+      </c>
       <c r="AM109" s="54"/>
       <c r="AN109" s="54"/>
       <c r="AO109" s="54"/>
@@ -12470,22 +12711,28 @@
       <c r="AU109" s="54"/>
       <c r="AV109">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="AW109" s="54"/>
-      <c r="AX109" s="54"/>
+      <c r="AX109" s="54">
+        <v>1</v>
+      </c>
       <c r="AY109" s="54"/>
-      <c r="AZ109" s="54"/>
+      <c r="AZ109" s="54">
+        <v>2</v>
+      </c>
       <c r="BA109" s="54">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="BB109" s="54"/>
       <c r="BC109">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="BD109" s="54"/>
+      <c r="BD109" s="54">
+        <v>7.5</v>
+      </c>
       <c r="BE109" s="54"/>
       <c r="BF109" s="54"/>
       <c r="BG109" s="54"/>
@@ -12519,22 +12766,30 @@
       <c r="AB110" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="AC110" s="47"/>
+      <c r="AC110" s="47" t="s">
+        <v>448</v>
+      </c>
       <c r="AD110" s="39">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-113</v>
       </c>
       <c r="AE110" s="48"/>
       <c r="AF110" s="48"/>
       <c r="AG110" s="54"/>
       <c r="AH110" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AI110" s="54"/>
-      <c r="AJ110" s="54"/>
+        <v>113</v>
+      </c>
+      <c r="AI110" s="54">
+        <v>69</v>
+      </c>
+      <c r="AJ110" s="54" t="s">
+        <v>451</v>
+      </c>
       <c r="AK110" s="54"/>
-      <c r="AL110" s="54"/>
+      <c r="AL110" s="54">
+        <v>12</v>
+      </c>
       <c r="AM110" s="54"/>
       <c r="AN110" s="54"/>
       <c r="AO110" s="54"/>
@@ -12546,22 +12801,30 @@
       <c r="AU110" s="54"/>
       <c r="AV110">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AW110" s="54"/>
-      <c r="AX110" s="54"/>
+        <v>32</v>
+      </c>
+      <c r="AW110" s="54">
+        <v>20</v>
+      </c>
+      <c r="AX110" s="54">
+        <v>2</v>
+      </c>
       <c r="AY110" s="54"/>
-      <c r="AZ110" s="54"/>
+      <c r="AZ110" s="54">
+        <v>1</v>
+      </c>
       <c r="BA110" s="54">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="BB110" s="54"/>
       <c r="BC110">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="BD110" s="54"/>
+      <c r="BD110" s="54">
+        <v>12</v>
+      </c>
       <c r="BE110" s="54"/>
       <c r="BF110" s="54"/>
       <c r="BG110" s="54"/>
@@ -12598,20 +12861,26 @@
       <c r="AC111" s="47"/>
       <c r="AD111" s="39">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-70</v>
       </c>
       <c r="AE111" s="48"/>
       <c r="AF111" s="48"/>
       <c r="AG111" s="54"/>
       <c r="AH111" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="AI111" s="54"/>
       <c r="AJ111" s="54"/>
-      <c r="AK111" s="54"/>
-      <c r="AL111" s="54"/>
-      <c r="AM111" s="54"/>
+      <c r="AK111" s="54" t="s">
+        <v>454</v>
+      </c>
+      <c r="AL111" s="54">
+        <v>50</v>
+      </c>
+      <c r="AM111" s="54">
+        <v>20</v>
+      </c>
       <c r="AN111" s="54"/>
       <c r="AO111" s="54"/>
       <c r="AP111" s="54"/>
@@ -12627,10 +12896,12 @@
       <c r="AW111" s="54"/>
       <c r="AX111" s="54"/>
       <c r="AY111" s="54"/>
-      <c r="AZ111" s="54"/>
+      <c r="AZ111" s="54">
+        <v>1</v>
+      </c>
       <c r="BA111" s="54">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BB111" s="54"/>
       <c r="BC111">
@@ -12750,19 +13021,27 @@
       <c r="AC113" s="47"/>
       <c r="AD113" s="39">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-3900</v>
       </c>
       <c r="AE113" s="48"/>
       <c r="AF113" s="48"/>
       <c r="AG113" s="54"/>
       <c r="AH113" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AI113" s="54"/>
-      <c r="AJ113" s="54"/>
-      <c r="AK113" s="54"/>
-      <c r="AL113" s="54"/>
+        <v>3900</v>
+      </c>
+      <c r="AI113" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ113" s="54" t="s">
+        <v>452</v>
+      </c>
+      <c r="AK113" s="96" t="s">
+        <v>220</v>
+      </c>
+      <c r="AL113" s="96">
+        <v>3900</v>
+      </c>
       <c r="AM113" s="54"/>
       <c r="AN113" s="54"/>
       <c r="AO113" s="54"/>
@@ -12826,20 +13105,30 @@
       <c r="AC114" s="47"/>
       <c r="AD114" s="39">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-127</v>
       </c>
       <c r="AE114" s="48"/>
       <c r="AF114" s="48"/>
       <c r="AG114" s="54"/>
       <c r="AH114" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AI114" s="54"/>
-      <c r="AJ114" s="54"/>
-      <c r="AK114" s="54"/>
-      <c r="AL114" s="54"/>
-      <c r="AM114" s="54"/>
+        <v>127</v>
+      </c>
+      <c r="AI114" s="54">
+        <v>67</v>
+      </c>
+      <c r="AJ114" s="54" t="s">
+        <v>395</v>
+      </c>
+      <c r="AK114" s="54" t="s">
+        <v>455</v>
+      </c>
+      <c r="AL114" s="54">
+        <v>30</v>
+      </c>
+      <c r="AM114" s="54">
+        <v>30</v>
+      </c>
       <c r="AN114" s="54"/>
       <c r="AO114" s="54"/>
       <c r="AP114" s="54"/>
@@ -12853,12 +13142,16 @@
         <v>0</v>
       </c>
       <c r="AW114" s="54"/>
-      <c r="AX114" s="54"/>
+      <c r="AX114" s="54">
+        <v>1</v>
+      </c>
       <c r="AY114" s="54"/>
-      <c r="AZ114" s="54"/>
+      <c r="AZ114" s="54">
+        <v>1</v>
+      </c>
       <c r="BA114" s="54">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="BB114" s="54"/>
       <c r="BC114">
@@ -12902,14 +13195,14 @@
       <c r="AC115" s="47"/>
       <c r="AD115" s="39">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-50</v>
       </c>
       <c r="AE115" s="48"/>
       <c r="AF115" s="48"/>
       <c r="AG115" s="54"/>
       <c r="AH115" s="49">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="AI115" s="54"/>
       <c r="AJ115" s="54"/>
@@ -12926,15 +13219,19 @@
       <c r="AU115" s="54"/>
       <c r="AV115">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AW115" s="54"/>
+        <v>50</v>
+      </c>
+      <c r="AW115" s="54">
+        <v>50</v>
+      </c>
       <c r="AX115" s="54"/>
       <c r="AY115" s="54"/>
-      <c r="AZ115" s="54"/>
+      <c r="AZ115" s="54">
+        <v>1</v>
+      </c>
       <c r="BA115" s="54">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BB115" s="54"/>
       <c r="BC115">
@@ -13904,7 +14201,7 @@
       <c r="Q130" s="21"/>
       <c r="R130" s="20"/>
       <c r="S130" s="18">
-        <f t="shared" ref="S130:S144" si="19">Q130-R130</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="U130" s="33"/>
@@ -13961,7 +14258,7 @@
       <c r="Q131" s="21"/>
       <c r="R131" s="20"/>
       <c r="S131" s="18">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="S131:S145" si="19">Q131-R131</f>
         <v>0</v>
       </c>
       <c r="U131" s="33"/>
@@ -14467,13 +14764,13 @@
         <v>0</v>
       </c>
       <c r="K140" s="12"/>
-      <c r="M140" s="85"/>
-      <c r="N140" s="85"/>
-      <c r="O140" s="85"/>
+      <c r="M140" s="16"/>
+      <c r="N140" s="16"/>
+      <c r="O140" s="16"/>
       <c r="P140" s="33"/>
-      <c r="Q140" s="86"/>
-      <c r="R140" s="84"/>
-      <c r="S140" s="87">
+      <c r="Q140" s="21"/>
+      <c r="R140" s="20"/>
+      <c r="S140" s="18">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
@@ -14752,13 +15049,16 @@
         <v>0</v>
       </c>
       <c r="K145" s="12"/>
-      <c r="M145" s="89"/>
-      <c r="N145" s="89"/>
-      <c r="O145" s="89"/>
-      <c r="P145" s="129"/>
-      <c r="Q145" s="89"/>
-      <c r="R145" s="89"/>
-      <c r="S145" s="89"/>
+      <c r="M145" s="85"/>
+      <c r="N145" s="85"/>
+      <c r="O145" s="85"/>
+      <c r="P145" s="33"/>
+      <c r="Q145" s="86"/>
+      <c r="R145" s="84"/>
+      <c r="S145" s="87">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
       <c r="U145" s="33"/>
       <c r="V145" s="33"/>
       <c r="W145" s="33"/>
@@ -14809,7 +15109,7 @@
       <c r="M146" s="89"/>
       <c r="N146" s="89"/>
       <c r="O146" s="89"/>
-      <c r="P146" s="89"/>
+      <c r="P146" s="129"/>
       <c r="Q146" s="89"/>
       <c r="R146" s="89"/>
       <c r="S146" s="89"/>
@@ -15149,6 +15449,7 @@
       <c r="Q152" s="89"/>
       <c r="R152" s="89"/>
       <c r="S152" s="89"/>
+      <c r="T152"/>
       <c r="X152" s="88"/>
       <c r="Y152" s="88"/>
       <c r="AA152" s="99"/>
@@ -15337,6 +15638,7 @@
       <c r="I157" s="82"/>
       <c r="J157" s="83"/>
       <c r="K157" s="84"/>
+      <c r="T157" s="85"/>
       <c r="AA157" s="90"/>
       <c r="AB157" s="91"/>
       <c r="AD157" s="91"/>
@@ -17610,13 +17912,6 @@
     <row r="384" spans="9:34" s="89" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I384" s="95"/>
       <c r="J384" s="96"/>
-      <c r="M384"/>
-      <c r="N384"/>
-      <c r="O384"/>
-      <c r="P384"/>
-      <c r="Q384" s="22"/>
-      <c r="R384" s="12"/>
-      <c r="S384" s="19"/>
       <c r="AA384" s="91"/>
       <c r="AB384" s="91"/>
       <c r="AD384" s="91"/>
@@ -17789,6 +18084,7 @@
       <c r="J394" s="96"/>
       <c r="K394" s="89"/>
       <c r="Q394" s="22"/>
+      <c r="R394" s="12"/>
       <c r="S394" s="19"/>
       <c r="T394" s="89"/>
       <c r="X394" s="32"/>
@@ -17924,6 +18220,7 @@
       <c r="K396" s="89"/>
       <c r="Q396" s="22"/>
       <c r="S396" s="19"/>
+      <c r="T396" s="89"/>
       <c r="X396" s="32"/>
       <c r="Y396" s="32"/>
       <c r="AA396" s="46"/>
@@ -18965,6 +19262,7 @@
     </row>
     <row r="413" spans="17:55" x14ac:dyDescent="0.25">
       <c r="Q413" s="22"/>
+      <c r="S413" s="19"/>
       <c r="X413" s="32"/>
       <c r="Y413" s="32"/>
       <c r="AA413" s="46"/>
@@ -20284,6 +20582,7 @@
       </c>
     </row>
     <row r="435" spans="17:55" x14ac:dyDescent="0.25">
+      <c r="Q435" s="22"/>
       <c r="X435" s="32"/>
       <c r="Y435" s="32"/>
       <c r="AA435" s="46"/>
@@ -30406,8 +30705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>